<commit_message>
Updated test framework code
</commit_message>
<xml_diff>
--- a/testData/user_data.xlsx
+++ b/testData/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiranjibi\PycharmProjects\LumaShop\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF85AF37-A80A-4091-BAD1-1484B9F942C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2331241A-EFD7-4DDB-98C3-F977902664F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4690" yWindow="250" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,16 +48,16 @@
     <t>Demo@8171</t>
   </si>
   <si>
-    <t>user03</t>
-  </si>
-  <si>
-    <t>tu03@maildrop.cc</t>
-  </si>
-  <si>
-    <t>tu04@maildrop.cc</t>
-  </si>
-  <si>
-    <t>user04</t>
+    <t>user09</t>
+  </si>
+  <si>
+    <t>user08</t>
+  </si>
+  <si>
+    <t>tu09@maildrop.cc</t>
+  </si>
+  <si>
+    <t>tu08@maildrop.cc</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,7 +424,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -438,10 +438,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
added reporting and screenshots embedding for failed test cases
</commit_message>
<xml_diff>
--- a/testData/user_data.xlsx
+++ b/testData/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiranjibi\PycharmProjects\LumaShop\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2331241A-EFD7-4DDB-98C3-F977902664F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FBEE74-F110-488C-B509-2B4572623EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4690" yWindow="250" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,16 +48,16 @@
     <t>Demo@8171</t>
   </si>
   <si>
-    <t>user09</t>
-  </si>
-  <si>
-    <t>user08</t>
-  </si>
-  <si>
-    <t>tu09@maildrop.cc</t>
-  </si>
-  <si>
-    <t>tu08@maildrop.cc</t>
+    <t>tu11@maildrop.cc</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>tu10@maildrop.cc</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,10 +421,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -438,10 +438,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>

</xml_diff>